<commit_message>
Neue Daten. Kleinere Verbesserungen (Logging).
</commit_message>
<xml_diff>
--- a/data/c19stats-ac-import.xlsx
+++ b/data/c19stats-ac-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/Projects/covid-19-statistics-aachen/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA497FA9-F61F-4E4C-B8E8-9A725E58EE1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C01F391-0C64-6C4C-87C9-2FD8033DFA9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -711,103 +711,257 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="4">
+        <v>44113</v>
+      </c>
+      <c r="B11" s="6">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C11" s="5">
+        <v>3027</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1515</v>
+      </c>
+      <c r="E11" s="5">
+        <v>109</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2664</v>
+      </c>
+      <c r="G11" s="5">
+        <v>254</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+      <c r="A12" s="4">
+        <v>44116</v>
+      </c>
+      <c r="B12" s="6">
+        <v>0.46875</v>
+      </c>
+      <c r="C12" s="5">
+        <v>3167</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1585</v>
+      </c>
+      <c r="E12" s="5">
+        <v>109</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2723</v>
+      </c>
+      <c r="G12" s="5">
+        <v>335</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="A13" s="4">
+        <v>44117</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C13" s="5">
+        <v>3188</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1594</v>
+      </c>
+      <c r="E13" s="5">
+        <v>109</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2772</v>
+      </c>
+      <c r="G13" s="5">
+        <v>307</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="4"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="A14" s="4">
+        <v>44118</v>
+      </c>
+      <c r="B14" s="6">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C14" s="5">
+        <v>3257</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1626</v>
+      </c>
+      <c r="E14" s="5">
+        <v>109</v>
+      </c>
+      <c r="F14" s="5">
+        <v>2806</v>
+      </c>
+      <c r="G14" s="5">
+        <v>342</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="A15" s="4">
+        <v>44119</v>
+      </c>
+      <c r="B15" s="6">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C15" s="5">
+        <v>3393</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1672</v>
+      </c>
+      <c r="E15" s="5">
+        <v>109</v>
+      </c>
+      <c r="F15" s="5">
+        <v>2845</v>
+      </c>
+      <c r="G15" s="5">
+        <v>439</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="A16" s="4">
+        <v>44120</v>
+      </c>
+      <c r="B16" s="6">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C16" s="5">
+        <v>3509</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1729</v>
+      </c>
+      <c r="E16" s="5">
+        <v>109</v>
+      </c>
+      <c r="F16" s="5">
+        <v>2891</v>
+      </c>
+      <c r="G16" s="5">
+        <v>509</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="A17" s="4">
+        <v>44123</v>
+      </c>
+      <c r="B17" s="6">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C17" s="5">
+        <v>3778</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1838</v>
+      </c>
+      <c r="E17" s="5">
+        <v>110</v>
+      </c>
+      <c r="F17" s="5">
+        <v>3016</v>
+      </c>
+      <c r="G17" s="5">
+        <v>652</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="A18" s="4">
+        <v>44124</v>
+      </c>
+      <c r="B18" s="6">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C18" s="5">
+        <v>3816</v>
+      </c>
+      <c r="D18" s="5">
+        <v>1855</v>
+      </c>
+      <c r="E18" s="5">
+        <v>110</v>
+      </c>
+      <c r="F18" s="5">
+        <v>3084</v>
+      </c>
+      <c r="G18" s="5">
+        <v>622</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="A19" s="4">
+        <v>44125</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.4375</v>
+      </c>
+      <c r="C19" s="5">
+        <v>3912</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1894</v>
+      </c>
+      <c r="E19" s="5">
+        <v>110</v>
+      </c>
+      <c r="F19" s="5">
+        <v>3157</v>
+      </c>
+      <c r="G19" s="5">
+        <v>645</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="A20" s="4">
+        <v>44126</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C20" s="5">
+        <v>4103</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1973</v>
+      </c>
+      <c r="E20" s="5">
+        <v>111</v>
+      </c>
+      <c r="F20" s="5">
+        <v>3237</v>
+      </c>
+      <c r="G20" s="5">
+        <v>755</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="4"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="A21" s="4">
+        <v>44127</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0.4375</v>
+      </c>
+      <c r="C21" s="5">
+        <v>4288</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2031</v>
+      </c>
+      <c r="E21" s="5">
+        <v>111</v>
+      </c>
+      <c r="F21" s="5">
+        <v>3330</v>
+      </c>
+      <c r="G21" s="5">
+        <v>847</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>

</xml_diff>

<commit_message>
Allgemeine Aktualisierung. Visualisierung um neues Diagramm erweitert.
</commit_message>
<xml_diff>
--- a/data/c19stats-ac-import.xlsx
+++ b/data/c19stats-ac-import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DATA/Projects/covid-19-statistics-aachen/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D31780-23EA-0C4D-B3FD-CAC7F0C95F2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA46D39-4119-324D-8C0C-579AD974B57A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="22580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -505,118 +505,104 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
-        <v>44137</v>
+        <v>44166</v>
       </c>
       <c r="B2" s="6">
-        <v>0.41666666666666669</v>
+        <v>0.46875</v>
       </c>
       <c r="C2" s="5">
-        <v>6061</v>
+        <v>10316</v>
       </c>
       <c r="D2" s="5">
-        <v>2699</v>
+        <v>4441</v>
       </c>
       <c r="E2" s="5">
-        <v>125</v>
+        <v>184</v>
       </c>
       <c r="F2" s="5">
-        <v>4610</v>
+        <v>8968</v>
       </c>
       <c r="G2" s="5">
-        <v>1326</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
-        <v>44138</v>
+        <v>44167</v>
       </c>
       <c r="B3" s="6">
-        <v>0.64583333333333337</v>
+        <v>0.42708333333333331</v>
       </c>
       <c r="C3" s="5">
-        <v>6153</v>
+        <v>10460</v>
       </c>
       <c r="D3" s="5">
-        <v>2743</v>
+        <v>4487</v>
       </c>
       <c r="E3" s="5">
-        <v>129</v>
+        <v>188</v>
       </c>
       <c r="F3" s="5">
-        <v>4966</v>
+        <v>9194</v>
       </c>
       <c r="G3" s="5">
-        <v>1058</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
-        <v>44139</v>
+        <v>44168</v>
       </c>
       <c r="B4" s="6">
-        <v>0.44791666666666669</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C4" s="5">
-        <v>6278</v>
+        <v>10605</v>
       </c>
       <c r="D4" s="5">
-        <v>2785</v>
+        <v>4550</v>
       </c>
       <c r="E4" s="5">
-        <v>130</v>
+        <v>191</v>
       </c>
       <c r="F4" s="5">
-        <v>5013</v>
+        <v>9314</v>
       </c>
       <c r="G4" s="5">
-        <v>1135</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
-        <v>44140</v>
+        <v>44169</v>
       </c>
       <c r="B5" s="6">
-        <v>0.38541666666666669</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C5" s="5">
-        <v>6519</v>
+        <v>10764</v>
       </c>
       <c r="D5" s="5">
-        <v>2873</v>
+        <v>4627</v>
       </c>
       <c r="E5" s="5">
-        <v>130</v>
+        <v>196</v>
       </c>
       <c r="F5" s="5">
-        <v>5166</v>
+        <v>9548</v>
       </c>
       <c r="G5" s="5">
-        <v>1223</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
-        <v>44141</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0.4375</v>
-      </c>
-      <c r="C6" s="5">
-        <v>6748</v>
-      </c>
-      <c r="D6" s="5">
-        <v>2957</v>
-      </c>
-      <c r="E6" s="5">
-        <v>132</v>
-      </c>
-      <c r="F6" s="5">
-        <v>5360</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1256</v>
-      </c>
+      <c r="A6" s="4"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>

</xml_diff>